<commit_message>
Convert to excel from multiple arb file
</commit_message>
<xml_diff>
--- a/example/intl.xlsx
+++ b/example/intl.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -25,6 +25,9 @@
     <t xml:space="preserve">en</t>
   </si>
   <si>
+    <t xml:space="preserve">pl</t>
+  </si>
+  <si>
     <t xml:space="preserve">@@locale</t>
   </si>
   <si>
@@ -34,16 +37,37 @@
     <t xml:space="preserve">LLC</t>
   </si>
   <si>
+    <t xml:space="preserve">S.A.</t>
+  </si>
+  <si>
     <t xml:space="preserve">red_color</t>
   </si>
   <si>
     <t xml:space="preserve">Red</t>
   </si>
   <si>
+    <t xml:space="preserve">Czerwony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
     <t xml:space="preserve">orange_color</t>
   </si>
   <si>
     <t xml:space="preserve">Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomarańczowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pink_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Różowy</t>
   </si>
 </sst>
 </file>
@@ -292,6 +316,7 @@
     <col min="2" max="2" width="13.29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -307,37 +332,68 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>